<commit_message>
I didn't commit in too long. Sorry.
</commit_message>
<xml_diff>
--- a/units/comparison.xlsx
+++ b/units/comparison.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/deception/units/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="505" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8F5AC8-37DA-4054-AC10-A04816D1D51A}"/>
+  <xr:revisionPtr revIDLastSave="1016" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCAAD074-73FE-4F1B-B59E-9F2BF4575F9D}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12186" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit Value Calculation" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="102">
   <si>
     <t>race</t>
   </si>
@@ -234,13 +235,121 @@
   </si>
   <si>
     <t>gossamer</t>
+  </si>
+  <si>
+    <t>hitpoints</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>experience_next</t>
+  </si>
+  <si>
+    <t>How much XP this unit requires to level up</t>
+  </si>
+  <si>
+    <t>defense_deep_water</t>
+  </si>
+  <si>
+    <t>defense_shallow_water</t>
+  </si>
+  <si>
+    <t>defense_flat</t>
+  </si>
+  <si>
+    <t>defense_sand</t>
+  </si>
+  <si>
+    <t>defense_forest</t>
+  </si>
+  <si>
+    <t>defense_hills</t>
+  </si>
+  <si>
+    <t>defense_mountains</t>
+  </si>
+  <si>
+    <t>defense_village</t>
+  </si>
+  <si>
+    <t>defense_castle</t>
+  </si>
+  <si>
+    <t>defense_cave</t>
+  </si>
+  <si>
+    <t>defense_frozen</t>
+  </si>
+  <si>
+    <t>defense_unwalkable</t>
+  </si>
+  <si>
+    <t>defense_fungus</t>
+  </si>
+  <si>
+    <t>defense_impassable</t>
+  </si>
+  <si>
+    <t>resistance_blade</t>
+  </si>
+  <si>
+    <t>resistance_pierce</t>
+  </si>
+  <si>
+    <t>resistance_impact</t>
+  </si>
+  <si>
+    <t>resistance_fire</t>
+  </si>
+  <si>
+    <t>resistance_cold</t>
+  </si>
+  <si>
+    <t>resistance_arcane</t>
+  </si>
+  <si>
+    <t>damage_melee</t>
+  </si>
+  <si>
+    <t>damage_ranged</t>
+  </si>
+  <si>
+    <t>defense_coastal_reef</t>
+  </si>
+  <si>
+    <t>defense_swamp</t>
+  </si>
+  <si>
+    <t>higher is better</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>FILL THIS COLUMN</t>
+  </si>
+  <si>
+    <t>attribute value</t>
+  </si>
+  <si>
+    <t>sums</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,13 +365,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -277,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,6 +437,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,6 +507,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,10 +775,628 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90CC9FD-DE67-4ACC-A92F-D5EB853B51FF}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="38.64453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.29296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.8203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.8203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.8203125" customWidth="1"/>
+    <col min="6" max="6" width="8.9375" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="B1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
+        <v>5</v>
+      </c>
+      <c r="E2" s="17">
+        <f>D2*C2</f>
+        <v>5</v>
+      </c>
+      <c r="F2" s="18">
+        <f>E2</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="14">
+        <f>SUM(F2:F3)</f>
+        <v>27</v>
+      </c>
+      <c r="H2" s="22">
+        <f>G4/G2</f>
+        <v>14.392592592592594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="16">
+        <v>44</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="17">
+        <f>D3*C3</f>
+        <v>22</v>
+      </c>
+      <c r="F3" s="18">
+        <f t="shared" ref="F3" si="0">E3</f>
+        <v>22</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="16">
+        <v>29</v>
+      </c>
+      <c r="D4" s="19">
+        <v>4</v>
+      </c>
+      <c r="E4" s="17">
+        <f>D4*C4</f>
+        <v>116</v>
+      </c>
+      <c r="F4" s="20">
+        <f>SUM(E4:E7)</f>
+        <v>341</v>
+      </c>
+      <c r="G4" s="14">
+        <f>SUM(F4:F29)</f>
+        <v>388.6</v>
+      </c>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="16">
+        <v>20</v>
+      </c>
+      <c r="D5" s="19">
+        <v>6</v>
+      </c>
+      <c r="E5" s="17">
+        <f>D5*C5</f>
+        <v>120</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="16">
+        <v>9</v>
+      </c>
+      <c r="D6" s="19">
+        <v>5</v>
+      </c>
+      <c r="E6" s="17">
+        <f>D6*C6</f>
+        <v>45</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="B7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16">
+        <v>6</v>
+      </c>
+      <c r="D7" s="19">
+        <v>10</v>
+      </c>
+      <c r="E7" s="17">
+        <f>D7*C7</f>
+        <v>60</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="16">
+        <v>60</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="17">
+        <f>D8*C8</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="20">
+        <f>SUM(E8:E23)</f>
+        <v>17.599999999999998</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="16">
+        <v>40</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="17">
+        <f>D9*C9</f>
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="16">
+        <v>30</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="E10" s="17">
+        <f>D10*C10</f>
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="17">
+        <f>D11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="16">
+        <v>40</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="17">
+        <f>D12*C12</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="16">
+        <v>50</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="E13" s="17">
+        <f>D13*C13</f>
+        <v>2</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="16">
+        <v>20</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="17">
+        <f>D14*C14</f>
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="16">
+        <v>40</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="17">
+        <f>D15*C15</f>
+        <v>0.4</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="16">
+        <v>50</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="17">
+        <f>D16*C16</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="17">
+        <f>D17*C17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="16">
+        <v>60</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="E18" s="17">
+        <f>D18*C18</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="16">
+        <v>30</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="E19" s="17">
+        <f>D19*C19</f>
+        <v>0.6</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="16">
+        <v>20</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="17">
+        <f>D20*C20</f>
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="16">
+        <v>30</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="E21" s="17">
+        <f>D21*C21</f>
+        <v>0.6</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
+      </c>
+      <c r="D22" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="E22" s="17">
+        <f>D22*C22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="16">
+        <v>60</v>
+      </c>
+      <c r="D23" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="E23" s="17">
+        <f>D23*C23</f>
+        <v>2.4</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="16">
+        <v>100</v>
+      </c>
+      <c r="D24" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E24" s="17">
+        <f>D24*C24</f>
+        <v>5</v>
+      </c>
+      <c r="F24" s="20">
+        <f>SUM(E24:E29)</f>
+        <v>30</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="16">
+        <v>100</v>
+      </c>
+      <c r="D25" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E25" s="17">
+        <f>D25*C25</f>
+        <v>5</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="16">
+        <v>100</v>
+      </c>
+      <c r="D26" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E26" s="17">
+        <f>D26*C26</f>
+        <v>5</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="16">
+        <v>100</v>
+      </c>
+      <c r="D27" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E27" s="17">
+        <f>D27*C27</f>
+        <v>5</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="16">
+        <v>100</v>
+      </c>
+      <c r="D28" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E28" s="17">
+        <f>D28*C28</f>
+        <v>5</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="16">
+        <v>100</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="E29" s="17">
+        <f>D29*C29</f>
+        <v>5</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="G4:G29"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H29"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A8:A23"/>
+    <mergeCell ref="F8:F23"/>
+    <mergeCell ref="F24:F29"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>